<commit_message>
Commit multiple versions of MVPA preprocessing.
Clean up stuff from Talk Shop presentation.
</commit_message>
<xml_diff>
--- a/scripts/create_ancova_dset.xlsx
+++ b/scripts/create_ancova_dset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/netapp/MyersLab/Dave/Cthulhu/data/Cthulhu-fMRI/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/netapp-1/Research/MyersLab/Dave/Cthulhu/data/Cthulhu-fMRI/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3527AF-313F-4848-B6D9-88CEDCBF3CB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4418B76C-9A4F-CC41-8E8A-A212082AB9E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="4120" windowWidth="44280" windowHeight="24680" xr2:uid="{97CCA437-E5A6-424B-B528-D25800BA69B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="178">
   <si>
     <t>Subj</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>cth9/cth9.preproc/'stats.9+tlrc[13]' \</t>
+  </si>
+  <si>
+    <t>Step</t>
   </si>
 </sst>
 </file>
@@ -942,18 +945,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0121A1-E55E-DE40-B952-A4B1A7C4199C}">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D153"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -964,10 +967,13 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -977,11 +983,14 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -991,14 +1000,17 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1008,14 +1020,17 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1025,13 +1040,16 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1041,14 +1059,17 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1058,14 +1079,17 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1075,14 +1099,17 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1092,14 +1119,17 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1109,14 +1139,17 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1126,14 +1159,17 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1143,14 +1179,17 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1160,14 +1199,17 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
         <v>120</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1177,14 +1219,17 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1194,14 +1239,17 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1211,14 +1259,17 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1228,14 +1279,17 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1245,14 +1299,17 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1262,14 +1319,17 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1279,14 +1339,17 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1296,14 +1359,17 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1313,14 +1379,17 @@
       <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1330,14 +1399,17 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1347,14 +1419,17 @@
       <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1364,14 +1439,17 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1381,11 +1459,14 @@
       <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1395,11 +1476,14 @@
       <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1409,11 +1493,14 @@
       <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1423,11 +1510,14 @@
       <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1437,11 +1527,14 @@
       <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1451,11 +1544,14 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1465,11 +1561,14 @@
       <c r="C32" t="s">
         <v>22</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1479,11 +1578,14 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1493,11 +1595,14 @@
       <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1507,11 +1612,14 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1521,11 +1629,14 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1535,11 +1646,14 @@
       <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1549,11 +1663,14 @@
       <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1563,11 +1680,14 @@
       <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1577,11 +1697,14 @@
       <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1591,11 +1714,14 @@
       <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1605,11 +1731,14 @@
       <c r="C42" t="s">
         <v>22</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -1619,11 +1748,14 @@
       <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1633,11 +1765,14 @@
       <c r="C44" t="s">
         <v>22</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1647,11 +1782,14 @@
       <c r="C45" t="s">
         <v>22</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -1661,11 +1799,14 @@
       <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -1675,11 +1816,14 @@
       <c r="C47" t="s">
         <v>22</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1689,11 +1833,14 @@
       <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1703,11 +1850,14 @@
       <c r="C49" t="s">
         <v>22</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1717,11 +1867,14 @@
       <c r="C50" t="s">
         <v>22</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1731,11 +1884,14 @@
       <c r="C51" t="s">
         <v>22</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1745,11 +1901,14 @@
       <c r="C52" t="s">
         <v>22</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -1759,11 +1918,14 @@
       <c r="C53" t="s">
         <v>22</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1773,11 +1935,14 @@
       <c r="C54" t="s">
         <v>22</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1787,11 +1952,14 @@
       <c r="C55" t="s">
         <v>22</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1801,11 +1969,14 @@
       <c r="C56" t="s">
         <v>22</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56">
+        <v>5</v>
+      </c>
+      <c r="E56" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1815,11 +1986,14 @@
       <c r="C57" t="s">
         <v>22</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -1829,11 +2003,14 @@
       <c r="C58" t="s">
         <v>22</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1843,11 +2020,14 @@
       <c r="C59" t="s">
         <v>22</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1857,11 +2037,14 @@
       <c r="C60" t="s">
         <v>22</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1871,11 +2054,14 @@
       <c r="C61" t="s">
         <v>22</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1885,11 +2071,14 @@
       <c r="C62" t="s">
         <v>22</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1899,11 +2088,14 @@
       <c r="C63" t="s">
         <v>22</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1913,11 +2105,14 @@
       <c r="C64" t="s">
         <v>22</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1927,11 +2122,14 @@
       <c r="C65" t="s">
         <v>22</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65">
+        <v>7</v>
+      </c>
+      <c r="E65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -1941,11 +2139,14 @@
       <c r="C66" t="s">
         <v>22</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -1955,11 +2156,14 @@
       <c r="C67" t="s">
         <v>22</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -1969,11 +2173,14 @@
       <c r="C68" t="s">
         <v>22</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -1983,11 +2190,14 @@
       <c r="C69" t="s">
         <v>22</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1997,11 +2207,14 @@
       <c r="C70" t="s">
         <v>22</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2011,11 +2224,14 @@
       <c r="C71" t="s">
         <v>22</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -2025,11 +2241,14 @@
       <c r="C72" t="s">
         <v>22</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72">
+        <v>5</v>
+      </c>
+      <c r="E72" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -2039,11 +2258,14 @@
       <c r="C73" t="s">
         <v>22</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73">
+        <v>7</v>
+      </c>
+      <c r="E73" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2053,11 +2275,14 @@
       <c r="C74" t="s">
         <v>22</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2067,11 +2292,14 @@
       <c r="C75" t="s">
         <v>22</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2081,11 +2309,14 @@
       <c r="C76" t="s">
         <v>22</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2095,11 +2326,14 @@
       <c r="C77" t="s">
         <v>22</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -2109,11 +2343,14 @@
       <c r="C78" t="s">
         <v>23</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -2123,11 +2360,14 @@
       <c r="C79" t="s">
         <v>23</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
@@ -2137,11 +2377,14 @@
       <c r="C80" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
         <v>1</v>
       </c>
@@ -2151,11 +2394,14 @@
       <c r="C81" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81">
+        <v>7</v>
+      </c>
+      <c r="E81" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2165,11 +2411,14 @@
       <c r="C82" t="s">
         <v>23</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -2179,11 +2428,14 @@
       <c r="C83" t="s">
         <v>23</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
         <v>7</v>
       </c>
@@ -2193,11 +2445,14 @@
       <c r="C84" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84">
+        <v>5</v>
+      </c>
+      <c r="E84" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
         <v>7</v>
       </c>
@@ -2207,11 +2462,14 @@
       <c r="C85" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85">
+        <v>7</v>
+      </c>
+      <c r="E85" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2221,11 +2479,14 @@
       <c r="C86" t="s">
         <v>23</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2235,11 +2496,14 @@
       <c r="C87" t="s">
         <v>23</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="E87" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
         <v>8</v>
       </c>
@@ -2249,11 +2513,14 @@
       <c r="C88" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
         <v>8</v>
       </c>
@@ -2263,11 +2530,14 @@
       <c r="C89" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89">
+        <v>7</v>
+      </c>
+      <c r="E89" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -2277,11 +2547,14 @@
       <c r="C90" t="s">
         <v>23</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -2291,11 +2564,14 @@
       <c r="C91" t="s">
         <v>23</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
         <v>9</v>
       </c>
@@ -2305,11 +2581,14 @@
       <c r="C92" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="E92" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
         <v>9</v>
       </c>
@@ -2319,11 +2598,14 @@
       <c r="C93" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93">
+        <v>7</v>
+      </c>
+      <c r="E93" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -2333,11 +2615,14 @@
       <c r="C94" t="s">
         <v>23</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -2347,11 +2632,14 @@
       <c r="C95" t="s">
         <v>23</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
         <v>10</v>
       </c>
@@ -2361,11 +2649,14 @@
       <c r="C96" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96">
+        <v>5</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
         <v>10</v>
       </c>
@@ -2375,11 +2666,14 @@
       <c r="C97" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97">
+        <v>7</v>
+      </c>
+      <c r="E97" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -2389,11 +2683,14 @@
       <c r="C98" t="s">
         <v>23</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -2403,11 +2700,14 @@
       <c r="C99" t="s">
         <v>23</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
         <v>11</v>
       </c>
@@ -2417,11 +2717,14 @@
       <c r="C100" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100">
+        <v>5</v>
+      </c>
+      <c r="E100" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
         <v>11</v>
       </c>
@@ -2431,11 +2734,14 @@
       <c r="C101" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -2445,11 +2751,14 @@
       <c r="C102" t="s">
         <v>23</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -2459,11 +2768,14 @@
       <c r="C103" t="s">
         <v>23</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103">
+        <v>3</v>
+      </c>
+      <c r="E103" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
         <v>12</v>
       </c>
@@ -2473,11 +2785,14 @@
       <c r="C104" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
         <v>12</v>
       </c>
@@ -2487,11 +2802,14 @@
       <c r="C105" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -2501,11 +2819,14 @@
       <c r="C106" t="s">
         <v>23</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -2515,11 +2836,14 @@
       <c r="C107" t="s">
         <v>23</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107">
+        <v>3</v>
+      </c>
+      <c r="E107" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
         <v>13</v>
       </c>
@@ -2529,11 +2853,14 @@
       <c r="C108" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108">
+        <v>5</v>
+      </c>
+      <c r="E108" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
         <v>13</v>
       </c>
@@ -2543,11 +2870,14 @@
       <c r="C109" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109">
+        <v>7</v>
+      </c>
+      <c r="E109" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>14</v>
       </c>
@@ -2557,11 +2887,14 @@
       <c r="C110" t="s">
         <v>23</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>14</v>
       </c>
@@ -2571,11 +2904,14 @@
       <c r="C111" t="s">
         <v>23</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111">
+        <v>3</v>
+      </c>
+      <c r="E111" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
         <v>14</v>
       </c>
@@ -2585,11 +2921,14 @@
       <c r="C112" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
         <v>14</v>
       </c>
@@ -2599,11 +2938,14 @@
       <c r="C113" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113">
+        <v>7</v>
+      </c>
+      <c r="E113" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -2613,11 +2955,14 @@
       <c r="C114" t="s">
         <v>23</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -2627,11 +2972,14 @@
       <c r="C115" t="s">
         <v>23</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
         <v>2</v>
       </c>
@@ -2641,11 +2989,14 @@
       <c r="C116" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
         <v>2</v>
       </c>
@@ -2655,11 +3006,14 @@
       <c r="C117" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117">
+        <v>7</v>
+      </c>
+      <c r="E117" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>15</v>
       </c>
@@ -2669,11 +3023,14 @@
       <c r="C118" t="s">
         <v>23</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>15</v>
       </c>
@@ -2683,11 +3040,14 @@
       <c r="C119" t="s">
         <v>23</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="E119" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
         <v>15</v>
       </c>
@@ -2697,11 +3057,14 @@
       <c r="C120" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120">
+        <v>5</v>
+      </c>
+      <c r="E120" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
         <v>15</v>
       </c>
@@ -2711,11 +3074,14 @@
       <c r="C121" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121">
+        <v>7</v>
+      </c>
+      <c r="E121" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>16</v>
       </c>
@@ -2725,11 +3091,14 @@
       <c r="C122" t="s">
         <v>23</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>16</v>
       </c>
@@ -2739,11 +3108,14 @@
       <c r="C123" t="s">
         <v>23</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123">
+        <v>3</v>
+      </c>
+      <c r="E123" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
         <v>16</v>
       </c>
@@ -2753,11 +3125,14 @@
       <c r="C124" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124">
+        <v>5</v>
+      </c>
+      <c r="E124" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
         <v>16</v>
       </c>
@@ -2767,11 +3142,14 @@
       <c r="C125" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125">
+        <v>7</v>
+      </c>
+      <c r="E125" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -2781,11 +3159,14 @@
       <c r="C126" t="s">
         <v>23</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -2795,11 +3176,14 @@
       <c r="C127" t="s">
         <v>23</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127">
+        <v>3</v>
+      </c>
+      <c r="E127" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
         <v>17</v>
       </c>
@@ -2809,11 +3193,14 @@
       <c r="C128" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128">
+        <v>5</v>
+      </c>
+      <c r="E128" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
         <v>17</v>
       </c>
@@ -2823,11 +3210,14 @@
       <c r="C129" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129">
+        <v>7</v>
+      </c>
+      <c r="E129" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>18</v>
       </c>
@@ -2837,11 +3227,14 @@
       <c r="C130" t="s">
         <v>23</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -2851,11 +3244,14 @@
       <c r="C131" t="s">
         <v>23</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
         <v>18</v>
       </c>
@@ -2865,11 +3261,14 @@
       <c r="C132" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132">
+        <v>5</v>
+      </c>
+      <c r="E132" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
         <v>18</v>
       </c>
@@ -2879,11 +3278,14 @@
       <c r="C133" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133">
+        <v>7</v>
+      </c>
+      <c r="E133" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -2893,11 +3295,14 @@
       <c r="C134" t="s">
         <v>23</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>19</v>
       </c>
@@ -2907,11 +3312,14 @@
       <c r="C135" t="s">
         <v>23</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135">
+        <v>3</v>
+      </c>
+      <c r="E135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
         <v>19</v>
       </c>
@@ -2921,11 +3329,14 @@
       <c r="C136" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136">
+        <v>5</v>
+      </c>
+      <c r="E136" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
         <v>19</v>
       </c>
@@ -2935,11 +3346,14 @@
       <c r="C137" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137">
+        <v>7</v>
+      </c>
+      <c r="E137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>3</v>
       </c>
@@ -2949,11 +3363,14 @@
       <c r="C138" t="s">
         <v>23</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>3</v>
       </c>
@@ -2963,11 +3380,14 @@
       <c r="C139" t="s">
         <v>23</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139">
+        <v>3</v>
+      </c>
+      <c r="E139" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
         <v>3</v>
       </c>
@@ -2977,11 +3397,14 @@
       <c r="C140" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140">
+        <v>5</v>
+      </c>
+      <c r="E140" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
         <v>3</v>
       </c>
@@ -2991,11 +3414,14 @@
       <c r="C141" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141">
+        <v>7</v>
+      </c>
+      <c r="E141" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -3005,11 +3431,14 @@
       <c r="C142" t="s">
         <v>23</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>4</v>
       </c>
@@ -3019,11 +3448,14 @@
       <c r="C143" t="s">
         <v>23</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
         <v>4</v>
       </c>
@@ -3033,11 +3465,14 @@
       <c r="C144" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144">
+        <v>5</v>
+      </c>
+      <c r="E144" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
         <v>4</v>
       </c>
@@ -3047,11 +3482,14 @@
       <c r="C145" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145">
+        <v>7</v>
+      </c>
+      <c r="E145" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -3061,11 +3499,14 @@
       <c r="C146" t="s">
         <v>23</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -3075,11 +3516,14 @@
       <c r="C147" t="s">
         <v>23</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147">
+        <v>3</v>
+      </c>
+      <c r="E147" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
         <v>5</v>
       </c>
@@ -3089,11 +3533,14 @@
       <c r="C148" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148">
+        <v>5</v>
+      </c>
+      <c r="E148" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
         <v>5</v>
       </c>
@@ -3103,11 +3550,14 @@
       <c r="C149" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149">
+        <v>7</v>
+      </c>
+      <c r="E149" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -3117,11 +3567,14 @@
       <c r="C150" t="s">
         <v>23</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -3131,11 +3584,14 @@
       <c r="C151" t="s">
         <v>23</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151">
+        <v>3</v>
+      </c>
+      <c r="E151" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
         <v>6</v>
       </c>
@@ -3145,11 +3601,14 @@
       <c r="C152" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152">
+        <v>5</v>
+      </c>
+      <c r="E152" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:5">
       <c r="A153" s="3" t="s">
         <v>6</v>
       </c>
@@ -3159,12 +3618,15 @@
       <c r="C153" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153">
+        <v>7</v>
+      </c>
+      <c r="E153" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D77">
+  <sortState ref="A2:E77">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>